<commit_message>
Framework changes adding screenshot
</commit_message>
<xml_diff>
--- a/src/main/resources/sysExcel.xlsx
+++ b/src/main/resources/sysExcel.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>Module</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -31,6 +34,12 @@
     <t>password</t>
   </si>
   <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>SignUp</t>
+  </si>
+  <si>
     <t>Vinay</t>
   </si>
   <si>
@@ -41,6 +50,12 @@
   </si>
   <si>
     <t>asdf@1234</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>This is a required field.</t>
   </si>
 </sst>
 </file>
@@ -48,8 +63,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -78,74 +93,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -154,7 +101,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,6 +117,27 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -184,23 +152,70 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,13 +230,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,19 +344,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,55 +392,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,85 +404,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,6 +421,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -428,6 +458,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -438,21 +494,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -472,32 +513,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -511,142 +526,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1011,19 +1026,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="3" max="3" width="15.1" customWidth="1"/>
-    <col min="4" max="4" width="14.9" customWidth="1"/>
+    <col min="4" max="4" width="15.1" customWidth="1"/>
+    <col min="5" max="5" width="14.9" customWidth="1"/>
+    <col min="7" max="7" width="17.8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1039,28 +1055,56 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="vinay@codilar.com"/>
-    <hyperlink ref="E2" r:id="rId2" display="asdf@1234"/>
+    <hyperlink ref="E2" r:id="rId1" display="vinay@codilar.com"/>
+    <hyperlink ref="F2" r:id="rId2" display="asdf@1234"/>
+    <hyperlink ref="E3" r:id="rId1" display="vinay@codilar.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="asdf@1234"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Extent report framework changes
</commit_message>
<xml_diff>
--- a/src/main/resources/sysExcel.xlsx
+++ b/src/main/resources/sysExcel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Module</t>
   </si>
@@ -64,9 +64,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -86,7 +86,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -95,13 +95,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,35 +109,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -152,22 +116,81 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -175,16 +198,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,29 +220,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -230,13 +230,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,13 +392,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,151 +404,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,41 +448,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -494,6 +459,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,144 +489,170 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -661,7 +661,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="6"/>
@@ -1088,6 +1088,12 @@
       </c>
       <c r="B3">
         <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Framework fixed the extent reports and Cross browser testing
</commit_message>
<xml_diff>
--- a/src/main/resources/sysExcel.xlsx
+++ b/src/main/resources/sysExcel.xlsx
@@ -63,10 +63,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -85,6 +85,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,9 +100,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -109,107 +175,33 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -220,6 +212,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -230,13 +230,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,169 +410,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,6 +421,60 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -442,23 +496,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -467,22 +506,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -497,171 +521,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">

</xml_diff>

<commit_message>
Set basic Framework and added another testCase to verify link
</commit_message>
<xml_diff>
--- a/src/main/resources/sysExcel.xlsx
+++ b/src/main/resources/sysExcel.xlsx
@@ -63,9 +63,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -85,6 +85,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -93,6 +144,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,66 +153,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,6 +167,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -184,14 +184,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,22 +220,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -230,37 +230,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,37 +350,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,6 +380,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -332,85 +410,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,7 +428,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -449,6 +449,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -463,17 +478,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,176 +521,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">

</xml_diff>

<commit_message>
Added Privacy Policy pageModel and updated excelUtils logic
</commit_message>
<xml_diff>
--- a/src/main/resources/sysExcel.xlsx
+++ b/src/main/resources/sysExcel.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>username</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>firstname</t>
   </si>
   <si>
     <t>lastname</t>
@@ -34,10 +31,13 @@
     <t>password</t>
   </si>
   <si>
-    <t>Error Message</t>
-  </si>
-  <si>
-    <t>SignUp</t>
+    <t>error_message</t>
+  </si>
+  <si>
+    <t>error_box</t>
+  </si>
+  <si>
+    <t>sign_up</t>
   </si>
   <si>
     <t>Vinay</t>
@@ -52,10 +52,13 @@
     <t>asdf@1234</t>
   </si>
   <si>
-    <t>Login</t>
+    <t>login</t>
   </si>
   <si>
     <t>This is a required field.</t>
+  </si>
+  <si>
+    <t>A login and a password are required.</t>
   </si>
 </sst>
 </file>
@@ -64,9 +67,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -79,6 +82,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -86,6 +97,68 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -93,7 +166,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -113,113 +223,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -230,25 +233,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,25 +311,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,121 +335,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,8 +430,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,194 +524,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1029,14 +1035,15 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="4" max="4" width="15.1" customWidth="1"/>
-    <col min="5" max="5" width="14.9" customWidth="1"/>
-    <col min="7" max="7" width="17.8" customWidth="1"/>
+    <col min="3" max="3" width="15.1" customWidth="1"/>
+    <col min="4" max="4" width="14.9" customWidth="1"/>
+    <col min="6" max="6" width="17.8" customWidth="1"/>
+    <col min="7" max="7" width="17.7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1062,23 +1069,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1086,31 +1090,31 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="vinay@codilar.com"/>
-    <hyperlink ref="F2" r:id="rId2" display="asdf@1234"/>
-    <hyperlink ref="E3" r:id="rId1" display="vinay@codilar.com"/>
-    <hyperlink ref="F3" r:id="rId2" display="asdf@1234"/>
+    <hyperlink ref="D2" r:id="rId1" display="vinay@codilar.com"/>
+    <hyperlink ref="E2" r:id="rId2" display="asdf@1234"/>
+    <hyperlink ref="D3" r:id="rId1" display="vinay@codilar.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="asdf@1234"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Add user invalid and valid login check & Added logs to project
</commit_message>
<xml_diff>
--- a/src/main/resources/sysExcel.xlsx
+++ b/src/main/resources/sysExcel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>features</t>
   </si>
@@ -37,6 +37,9 @@
     <t>error_box</t>
   </si>
   <si>
+    <t>alt_email</t>
+  </si>
+  <si>
     <t>sign_up</t>
   </si>
   <si>
@@ -52,13 +55,31 @@
     <t>asdf@1234</t>
   </si>
   <si>
-    <t>login</t>
+    <t>validLogin</t>
   </si>
   <si>
     <t>This is a required field.</t>
   </si>
   <si>
     <t>A login and a password are required.</t>
+  </si>
+  <si>
+    <t>invalidLogin</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>The account sign-in was incorrect or your account is disabled temporarily. Please wait and try again later.</t>
+  </si>
+  <si>
+    <t>emails</t>
+  </si>
+  <si>
+    <t>topintest@gmail.com</t>
+  </si>
+  <si>
+    <t>test#123</t>
   </si>
 </sst>
 </file>
@@ -66,10 +87,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -97,15 +118,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,6 +202,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -173,52 +239,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,19 +254,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,31 +392,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,127 +434,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,31 +451,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -485,21 +493,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -514,13 +507,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,142 +550,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1032,13 +1053,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="4" outlineLevelCol="7"/>
   <cols>
     <col min="3" max="3" width="15.1" customWidth="1"/>
     <col min="4" max="4" width="14.9" customWidth="1"/>
@@ -1046,7 +1067,7 @@
     <col min="7" max="7" width="17.7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1067,46 +1088,86 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1115,6 +1176,10 @@
     <hyperlink ref="E2" r:id="rId2" display="asdf@1234"/>
     <hyperlink ref="D3" r:id="rId1" display="vinay@codilar.com"/>
     <hyperlink ref="E3" r:id="rId2" display="asdf@1234"/>
+    <hyperlink ref="D4" r:id="rId3" display="abc@gmail.com" tooltip="mailto:abc@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId2" display="asdf@1234"/>
+    <hyperlink ref="D5" r:id="rId4" display="topintest@gmail.com"/>
+    <hyperlink ref="H5" r:id="rId1" display="vinay@codilar.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>